<commit_message>
added dissociation protocol and data corrections
</commit_message>
<xml_diff>
--- a/examples/spreadsheets/current/filled/Q4DemoSS2Metadata.xlsx
+++ b/examples/spreadsheets/current/filled/Q4DemoSS2Metadata.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hewgreen/Google Drive/metadata-schema/examples/spreadsheets/current/filled/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{019D07FD-5272-F040-8C2E-F09C2A7369B7}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{820533B8-805F-FA49-A6DA-5167E5CD88C8}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="25600" yWindow="460" windowWidth="25600" windowHeight="27480" firstSheet="6" activeTab="12" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="24660" yWindow="460" windowWidth="26540" windowHeight="20780" firstSheet="7" activeTab="15" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Project" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1145" uniqueCount="683">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1166" uniqueCount="693">
   <si>
     <t>A unique label for the project.</t>
   </si>
@@ -2084,13 +2084,43 @@
   </si>
   <si>
     <t>single cell sequencing process</t>
+  </si>
+  <si>
+    <t>no</t>
+  </si>
+  <si>
+    <t>R1.fastq.gz</t>
+  </si>
+  <si>
+    <t>R2.fastq.gz</t>
+  </si>
+  <si>
+    <t>fastq.gz</t>
+  </si>
+  <si>
+    <t>read2</t>
+  </si>
+  <si>
+    <t>sequence_process_file_1</t>
+  </si>
+  <si>
+    <t>dissociation_1</t>
+  </si>
+  <si>
+    <t>a FACS method to separate cells</t>
+  </si>
+  <si>
+    <t>fluorescence-activated cell sorting</t>
+  </si>
+  <si>
+    <t>EFO:0009108</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -2132,6 +2162,17 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF032F62"/>
+      <name val="Consolas"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="13"/>
+      <name val="Verdana"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="4">
     <fill>
@@ -2169,7 +2210,7 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -2182,6 +2223,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -2524,7 +2568,7 @@
   <dimension ref="A1:H6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J6" sqref="J6"/>
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2841,9 +2885,11 @@
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
-  <dimension ref="A1:O5"/>
+  <dimension ref="A1:O12"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A6" sqref="A6"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
@@ -3031,8 +3077,26 @@
         <v>4</v>
       </c>
     </row>
+    <row r="6" spans="1:15" ht="17" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>689</v>
+      </c>
+      <c r="B6" t="s">
+        <v>690</v>
+      </c>
+      <c r="G6" t="s">
+        <v>691</v>
+      </c>
+      <c r="H6" s="10" t="s">
+        <v>692</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15" ht="16" x14ac:dyDescent="0.2">
+      <c r="G12" s="9"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
 
@@ -3196,7 +3260,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0C00-000000000000}">
   <dimension ref="A1:AR6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="AA1" sqref="AA1"/>
     </sheetView>
   </sheetViews>
@@ -3731,7 +3795,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0D00-000000000000}">
   <dimension ref="A1:L6"/>
   <sheetViews>
-    <sheetView topLeftCell="G1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="K6" sqref="K6"/>
     </sheetView>
   </sheetViews>
@@ -4098,7 +4162,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0F00-000000000000}">
   <dimension ref="A1:A27"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
@@ -4500,8 +4564,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:AV6"/>
   <sheetViews>
-    <sheetView topLeftCell="Q1" workbookViewId="0">
-      <selection activeCell="Z6" sqref="Z6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="AR8" sqref="AR8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -5016,6 +5080,12 @@
       <c r="Z6" s="6" t="s">
         <v>664</v>
       </c>
+      <c r="AR6" t="s">
+        <v>683</v>
+      </c>
+      <c r="AS6" t="s">
+        <v>663</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -5026,8 +5096,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:AI6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="R13" sqref="R13"/>
+    <sheetView topLeftCell="O1" workbookViewId="0">
+      <selection activeCell="J4" sqref="J4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -5434,8 +5504,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:AE6"/>
   <sheetViews>
-    <sheetView topLeftCell="Z1" workbookViewId="0">
-      <selection activeCell="AE6" sqref="AE6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="AD6" sqref="AD6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -5781,6 +5851,12 @@
       <c r="B6" s="5" t="s">
         <v>665</v>
       </c>
+      <c r="E6">
+        <v>9606</v>
+      </c>
+      <c r="AD6" t="s">
+        <v>689</v>
+      </c>
       <c r="AE6" t="s">
         <v>674</v>
       </c>
@@ -5792,9 +5868,11 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
-  <dimension ref="A1:P5"/>
+  <dimension ref="A1:P7"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B29" sqref="B29"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
@@ -5978,6 +6056,58 @@
     <row r="5" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A5" s="3" t="s">
         <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A6" s="8" t="s">
+        <v>684</v>
+      </c>
+      <c r="B6" s="8" t="s">
+        <v>665</v>
+      </c>
+      <c r="C6" s="8" t="s">
+        <v>686</v>
+      </c>
+      <c r="E6" t="s">
+        <v>316</v>
+      </c>
+      <c r="F6" s="8">
+        <v>1</v>
+      </c>
+      <c r="N6" t="s">
+        <v>676</v>
+      </c>
+      <c r="O6" t="s">
+        <v>680</v>
+      </c>
+      <c r="P6" t="s">
+        <v>688</v>
+      </c>
+    </row>
+    <row r="7" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A7" s="8" t="s">
+        <v>685</v>
+      </c>
+      <c r="B7" s="8" t="s">
+        <v>665</v>
+      </c>
+      <c r="C7" s="8" t="s">
+        <v>686</v>
+      </c>
+      <c r="E7" t="s">
+        <v>687</v>
+      </c>
+      <c r="F7" s="8">
+        <v>1</v>
+      </c>
+      <c r="N7" t="s">
+        <v>676</v>
+      </c>
+      <c r="O7" t="s">
+        <v>680</v>
+      </c>
+      <c r="P7" t="s">
+        <v>688</v>
       </c>
     </row>
   </sheetData>

</xml_diff>